<commit_message>
updating with some report format changes
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,20 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpura\eclipse-workspace\DataDrivenAutomation\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{527CB3E7-C19A-41EA-B6E0-D98EDB10ADE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0B1E99D7-20FC-4FFA-ACF3-52E0B96C652A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6C7E03C6-9F52-4744-90B8-F52E53AA7AD7}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20760" windowHeight="11820" xr2:uid="{6C7E03C6-9F52-4744-90B8-F52E53AA7AD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Register" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:K6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -445,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969B1951-3EA0-4419-A14B-98E5B0D8ED8E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -492,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15603C32-4CDD-4FAD-A278-2103026788F8}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>